<commit_message>
+ Project 2 completed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rencita.Monteiro\Documents\UiPath\Rencita_Capstone_2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED64F487-1EBD-42C0-95FE-ACB9104F7964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7CBADE-078E-471C-AD7B-2A2FE5A86AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -216,6 +216,12 @@
   </si>
   <si>
     <t>ArrayOfMonths</t>
+  </si>
+  <si>
+    <t>InvalidCredentials</t>
+  </si>
+  <si>
+    <t>Username and password is incorrect</t>
   </si>
 </sst>
 </file>
@@ -594,7 +600,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -753,7 +759,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>

</xml_diff>